<commit_message>
Updates to many map files
Updated many map files to include 2020 Census Data. Also moved most shapefiles out of Github to solve for storage limits and speed. Files will be hosted in OneDrive
</commit_message>
<xml_diff>
--- a/glpverse.xlsx
+++ b/glpverse.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1c93cd8282dd62d7/GLP/glptools/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cflouisville-my.sharepoint.com/personal/harrisonk_cflouisville_org/Documents/Documents/R/glptools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="14_{EDA3E6BB-038D-4042-AB00-A94A8ED991AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{0C573821-EB5C-4F92-AA64-A7D563B18E39}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="14_{EDA3E6BB-038D-4042-AB00-A94A8ED991AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB711FBF-68B0-409A-8BBE-DB7F62E2EB97}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{816E9ECE-A864-44CD-8637-99336C589178}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{816E9ECE-A864-44CD-8637-99336C589178}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -579,10 +579,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -900,27 +899,27 @@
   <dimension ref="A1:W114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L34" sqref="L34"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.47265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.20703125" customWidth="1"/>
-    <col min="3" max="3" width="21.3125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="17.5234375" customWidth="1"/>
-    <col min="6" max="6" width="12.7890625" customWidth="1"/>
-    <col min="7" max="7" width="18.41796875" customWidth="1"/>
-    <col min="8" max="8" width="14.9453125" customWidth="1"/>
-    <col min="9" max="9" width="10.734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.1015625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.7890625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.41796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.21875" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="17.5546875" customWidth="1"/>
+    <col min="6" max="6" width="12.77734375" customWidth="1"/>
+    <col min="7" max="7" width="18.44140625" customWidth="1"/>
+    <col min="8" max="8" width="15" customWidth="1"/>
+    <col min="9" max="9" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -949,7 +948,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -965,17 +964,17 @@
       <c r="E2" t="s">
         <v>99</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="F2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1001,7 +1000,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1030,7 +1029,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1056,7 +1055,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1085,7 +1084,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1111,7 +1110,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1137,7 +1136,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1163,7 +1162,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1189,7 +1188,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1215,7 +1214,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1253,7 +1252,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -1294,7 +1293,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1326,7 +1325,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1361,7 +1360,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -1399,7 +1398,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -1443,7 +1442,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -1472,7 +1471,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -1507,7 +1506,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -1542,7 +1541,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>47</v>
       </c>
@@ -1568,7 +1567,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>47</v>
       </c>
@@ -1597,7 +1596,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>47</v>
       </c>
@@ -1623,7 +1622,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>52</v>
       </c>
@@ -1649,7 +1648,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>52</v>
       </c>
@@ -1675,7 +1674,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>52</v>
       </c>
@@ -1704,7 +1703,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>52</v>
       </c>
@@ -1733,7 +1732,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>52</v>
       </c>
@@ -1771,7 +1770,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>52</v>
       </c>
@@ -1803,7 +1802,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>52</v>
       </c>
@@ -1832,7 +1831,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>52</v>
       </c>
@@ -1864,7 +1863,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>52</v>
       </c>
@@ -1893,7 +1892,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>52</v>
       </c>
@@ -1931,7 +1930,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>52</v>
       </c>
@@ -1969,7 +1968,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>52</v>
       </c>
@@ -1998,7 +1997,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>66</v>
       </c>
@@ -2030,7 +2029,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>66</v>
       </c>
@@ -2056,7 +2055,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>66</v>
       </c>
@@ -2097,7 +2096,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>70</v>
       </c>
@@ -2126,7 +2125,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>70</v>
       </c>
@@ -2158,7 +2157,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>70</v>
       </c>
@@ -2193,7 +2192,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>70</v>
       </c>
@@ -2219,7 +2218,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>70</v>
       </c>
@@ -2245,7 +2244,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>70</v>
       </c>
@@ -2271,7 +2270,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>70</v>
       </c>
@@ -2297,7 +2296,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>70</v>
       </c>
@@ -2323,7 +2322,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>79</v>
       </c>
@@ -2361,7 +2360,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>79</v>
       </c>
@@ -2390,7 +2389,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>79</v>
       </c>
@@ -2428,7 +2427,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>79</v>
       </c>
@@ -2457,7 +2456,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>79</v>
       </c>
@@ -2483,7 +2482,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>86</v>
       </c>
@@ -2515,7 +2514,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>86</v>
       </c>
@@ -2541,7 +2540,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>86</v>
       </c>
@@ -2567,7 +2566,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>90</v>
       </c>
@@ -2602,7 +2601,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>90</v>
       </c>
@@ -2640,7 +2639,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>92</v>
       </c>
@@ -2669,7 +2668,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>92</v>
       </c>
@@ -2698,7 +2697,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>92</v>
       </c>
@@ -2727,7 +2726,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>92</v>
       </c>
@@ -2756,7 +2755,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>97</v>
       </c>
@@ -2827,7 +2826,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>97</v>
       </c>
@@ -2853,7 +2852,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>97</v>
       </c>
@@ -2885,7 +2884,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>97</v>
       </c>
@@ -2920,7 +2919,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>97</v>
       </c>
@@ -2949,7 +2948,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>97</v>
       </c>
@@ -2987,7 +2986,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>97</v>
       </c>
@@ -3016,7 +3015,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>97</v>
       </c>
@@ -3042,7 +3041,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>97</v>
       </c>
@@ -3068,7 +3067,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>97</v>
       </c>
@@ -3103,7 +3102,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>97</v>
       </c>
@@ -3129,7 +3128,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>97</v>
       </c>
@@ -3155,7 +3154,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>97</v>
       </c>
@@ -3181,7 +3180,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>97</v>
       </c>
@@ -3207,7 +3206,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>97</v>
       </c>
@@ -3233,7 +3232,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>28</v>
       </c>
@@ -3277,7 +3276,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>28</v>
       </c>
@@ -3303,7 +3302,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>144</v>
       </c>
@@ -3332,7 +3331,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>121</v>
       </c>
@@ -3358,7 +3357,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>121</v>
       </c>
@@ -3387,7 +3386,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>121</v>
       </c>
@@ -3416,7 +3415,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>121</v>
       </c>
@@ -3445,7 +3444,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>121</v>
       </c>
@@ -3471,7 +3470,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>121</v>
       </c>
@@ -3497,7 +3496,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>21</v>
       </c>
@@ -3526,7 +3525,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>21</v>
       </c>
@@ -3555,7 +3554,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>21</v>
       </c>
@@ -3587,7 +3586,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>21</v>
       </c>
@@ -3616,7 +3615,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>147</v>
       </c>
@@ -3654,7 +3653,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>147</v>
       </c>
@@ -3692,7 +3691,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>147</v>
       </c>
@@ -3730,7 +3729,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>152</v>
       </c>
@@ -3762,7 +3761,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>152</v>
       </c>
@@ -3791,7 +3790,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>152</v>
       </c>
@@ -3820,7 +3819,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>154</v>
       </c>
@@ -3852,7 +3851,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>154</v>
       </c>
@@ -3884,7 +3883,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>155</v>
       </c>
@@ -3916,7 +3915,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>165</v>
       </c>
@@ -3942,7 +3941,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>165</v>
       </c>
@@ -3968,7 +3967,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>165</v>
       </c>
@@ -3994,7 +3993,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>165</v>
       </c>
@@ -4020,7 +4019,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>165</v>
       </c>
@@ -4046,7 +4045,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>165</v>
       </c>
@@ -4075,7 +4074,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>165</v>
       </c>
@@ -4104,7 +4103,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>165</v>
       </c>
@@ -4133,7 +4132,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>165</v>
       </c>
@@ -4162,7 +4161,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>165</v>
       </c>
@@ -4191,7 +4190,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>165</v>
       </c>
@@ -4217,7 +4216,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>165</v>
       </c>
@@ -4243,7 +4242,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>165</v>
       </c>
@@ -4269,7 +4268,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>165</v>
       </c>
@@ -4295,7 +4294,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>165</v>
       </c>
@@ -4324,7 +4323,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>165</v>
       </c>
@@ -4350,7 +4349,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>64</v>
       </c>
@@ -4390,9 +4389,9 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>124</v>
       </c>
@@ -4400,7 +4399,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -4408,7 +4407,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -4416,7 +4415,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -4424,7 +4423,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -4432,7 +4431,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>43</v>
       </c>

</xml_diff>